<commit_message>
#22 - fix connection between HomePage/CalendarPage and EditToDoPage
</commit_message>
<xml_diff>
--- a/TimeManagementApp/Dao/tasks.xlsx
+++ b/TimeManagementApp/Dao/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WP Project (Milestone 2)\Window-TimeManagementApp\TimeManagementApp\Dao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E4A2B-66EF-48A3-87FD-A3ADCBD73628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C4A01-FCF7-4B07-864F-EBE2E0C85EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>TaskId</t>
   </si>
@@ -49,13 +49,13 @@
     <t>NoteId</t>
   </si>
   <si>
-    <t>Task One</t>
-  </si>
-  <si>
-    <t>1/1/2024 9:00:00 AM</t>
-  </si>
-  <si>
-    <t>Description of Task One</t>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>11/27/2024 9:25:00 AM</t>
+  </si>
+  <si>
+    <t>Task 1 description</t>
   </si>
   <si>
     <t>False</t>
@@ -67,151 +67,145 @@
     <t>Daily</t>
   </si>
   <si>
-    <t>12/31/2023 9:00:00 AM</t>
-  </si>
-  <si>
-    <t>Task Two</t>
-  </si>
-  <si>
-    <t>1/2/2024 10:00:00 AM</t>
-  </si>
-  <si>
-    <t>Description of Task Two</t>
+    <t>11/28/2024 8:55:00 AM</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>11/29/2024 1:14:00 PM</t>
+  </si>
+  <si>
+    <t>Task 2 description</t>
   </si>
   <si>
     <t>Weekly</t>
   </si>
   <si>
-    <t>1/1/2024 10:00:00 AM</t>
-  </si>
-  <si>
-    <t>Task Three</t>
-  </si>
-  <si>
-    <t>1/3/2024 11:00:00 AM</t>
-  </si>
-  <si>
-    <t>Description of Task Three</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>1/2/2024 11:00:00 AM</t>
-  </si>
-  <si>
-    <t>Task Four</t>
-  </si>
-  <si>
-    <t>1/4/2024 12:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Four</t>
+    <t>11/29/2024 12:45:00 PM</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>11/30/2024 5:08:00 PM</t>
+  </si>
+  <si>
+    <t>Task 3 description</t>
   </si>
   <si>
     <t>Monthly</t>
   </si>
   <si>
-    <t>1/3/2024 12:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Five</t>
-  </si>
-  <si>
-    <t>1/5/2024 1:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Five</t>
-  </si>
-  <si>
-    <t>Yearly</t>
-  </si>
-  <si>
-    <t>1/4/2024 1:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Six</t>
-  </si>
-  <si>
-    <t>1/6/2024 2:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Six</t>
-  </si>
-  <si>
-    <t>1/5/2024 2:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Seven</t>
-  </si>
-  <si>
-    <t>1/7/2024 3:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Seven</t>
-  </si>
-  <si>
-    <t>1/6/2024 3:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Nine</t>
-  </si>
-  <si>
-    <t>1/9/2024 5:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Nine</t>
-  </si>
-  <si>
-    <t>1/8/2024 5:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Ten</t>
-  </si>
-  <si>
-    <t>1/10/2024 6:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Ten</t>
-  </si>
-  <si>
-    <t>1/9/2024 6:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Eleven</t>
-  </si>
-  <si>
-    <t>1/11/2024 7:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Eleven</t>
-  </si>
-  <si>
-    <t>1/10/2024 7:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task Twelve</t>
-  </si>
-  <si>
-    <t>1/12/2024 8:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task Twelve</t>
-  </si>
-  <si>
-    <t>1/11/2024 8:00:00 PM</t>
-  </si>
-  <si>
-    <t>Task 13</t>
-  </si>
-  <si>
-    <t>1/13/2024 1:00:00 PM</t>
-  </si>
-  <si>
-    <t>Description of Task 13</t>
-  </si>
-  <si>
-    <t>1/12/2024 9:00:00 PM</t>
+    <t>11/30/2024 4:31:00 PM</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>12/1/2024 8:47:00 PM</t>
+  </si>
+  <si>
+    <t>Task 4 description</t>
+  </si>
+  <si>
+    <t>12/1/2024 8:10:00 PM</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>11/28/2024 11:13:00 AM</t>
+  </si>
+  <si>
+    <t>Task 5 description</t>
+  </si>
+  <si>
+    <t>11/28/2024 10:45:00 AM</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>11/29/2024 2:22:00 PM</t>
+  </si>
+  <si>
+    <t>Task 6 description</t>
+  </si>
+  <si>
+    <t>11/29/2024 1:57:00 PM</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>11/30/2024 7:05:00 PM</t>
+  </si>
+  <si>
+    <t>Task 7 description</t>
+  </si>
+  <si>
+    <t>11/30/2024 6:30:00 PM</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>12/1/2024 10:30:00 PM</t>
+  </si>
+  <si>
+    <t>Task 8 description</t>
+  </si>
+  <si>
+    <t>12/1/2024 9:55:00 PM</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>11/28/2024 10:50:00 AM</t>
+  </si>
+  <si>
+    <t>Task 9 description</t>
+  </si>
+  <si>
+    <t>11/28/2024 10:15:00 AM</t>
+  </si>
+  <si>
+    <t>Task 10</t>
+  </si>
+  <si>
+    <t>11/29/2024 3:41:00 PM</t>
+  </si>
+  <si>
+    <t>Task 10 description</t>
+  </si>
+  <si>
+    <t>11/29/2024 3:12:00 PM</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>11/30/2024 6:32:00 PM</t>
+  </si>
+  <si>
+    <t>Task 11 description</t>
+  </si>
+  <si>
+    <t>11/30/2024 6:00:00 PM</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>12/1/2024 9:19:00 PM</t>
+  </si>
+  <si>
+    <t>Task 12 description</t>
+  </si>
+  <si>
+    <t>12/1/2024 8:45:00 PM</t>
   </si>
 </sst>
 </file>
@@ -564,7 +558,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -624,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="0">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -644,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>19</v>
@@ -653,7 +647,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="0">
-        <v>102</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -673,7 +667,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>24</v>
@@ -682,7 +676,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="0">
-        <v>103</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -699,19 +693,19 @@
         <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" s="0">
-        <v>104</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -719,28 +713,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="I6" s="0">
-        <v>105</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -748,28 +742,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="I7" s="0">
-        <v>106</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -777,173 +771,173 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="E8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="I8" s="0">
-        <v>107</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="I9" s="0">
-        <v>109</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="E10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="I10" s="0">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I11" s="0">
-        <v>111</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="E12" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" s="0">
-        <v>112</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="I13" s="0">
-        <v>113</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#22 - reminder & repeat update task
</commit_message>
<xml_diff>
--- a/TimeManagementApp/Dao/tasks.xlsx
+++ b/TimeManagementApp/Dao/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WP Project (Milestone 2)\Window-TimeManagementApp\TimeManagementApp\Dao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C4A01-FCF7-4B07-864F-EBE2E0C85EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61CA7F-98D1-42B7-8A7A-ACA1190B5384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>TaskId</t>
   </si>
@@ -49,150 +49,123 @@
     <t>NoteId</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>11/27/2024 9:25:00 AM</t>
-  </si>
-  <si>
-    <t>Task 1 description</t>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>11/30/2024 5:08:00 PM</t>
+  </si>
+  <si>
+    <t>Task 3 description</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>12/3/2024 6:00:00 AM</t>
+  </si>
+  <si>
+    <t>Task 400</t>
+  </si>
+  <si>
+    <t>12/1/2024 8:47:00 PM</t>
+  </si>
+  <si>
+    <t>Description of Task 400</t>
+  </si>
+  <si>
     <t>True</t>
   </si>
   <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>11/28/2024 8:55:00 AM</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>11/29/2024 1:14:00 PM</t>
-  </si>
-  <si>
-    <t>Task 2 description</t>
+    <t>12/9/2024 6:00:00 AM</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>11/28/2024 11:13:00 AM</t>
+  </si>
+  <si>
+    <t>Task 5 description</t>
+  </si>
+  <si>
+    <t>1/1/2000 1:00:00 AM</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>11/29/2024 2:22:00 PM</t>
+  </si>
+  <si>
+    <t>Task 6 description</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>11/30/2024 7:05:00 PM</t>
+  </si>
+  <si>
+    <t>Task 7 description</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>12/1/2024 10:30:00 PM</t>
+  </si>
+  <si>
+    <t>Task 8 description</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>12/1/2024 9:55:00 PM</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>11/28/2024 10:50:00 AM</t>
+  </si>
+  <si>
+    <t>Task 9 description</t>
+  </si>
+  <si>
+    <t>11/28/2024 10:15:00 AM</t>
+  </si>
+  <si>
+    <t>Task 10</t>
+  </si>
+  <si>
+    <t>11/29/2024 3:41:00 PM</t>
+  </si>
+  <si>
+    <t>Task 10 description</t>
+  </si>
+  <si>
+    <t>11/29/2024 3:12:00 PM</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>11/30/2024 6:32:00 PM</t>
+  </si>
+  <si>
+    <t>Task 11 description</t>
   </si>
   <si>
     <t>Weekly</t>
   </si>
   <si>
-    <t>11/29/2024 12:45:00 PM</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>11/30/2024 5:08:00 PM</t>
-  </si>
-  <si>
-    <t>Task 3 description</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>11/30/2024 4:31:00 PM</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>12/1/2024 8:47:00 PM</t>
-  </si>
-  <si>
-    <t>Task 4 description</t>
-  </si>
-  <si>
-    <t>12/1/2024 8:10:00 PM</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>11/28/2024 11:13:00 AM</t>
-  </si>
-  <si>
-    <t>Task 5 description</t>
-  </si>
-  <si>
-    <t>11/28/2024 10:45:00 AM</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>11/29/2024 2:22:00 PM</t>
-  </si>
-  <si>
-    <t>Task 6 description</t>
-  </si>
-  <si>
-    <t>11/29/2024 1:57:00 PM</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>11/30/2024 7:05:00 PM</t>
-  </si>
-  <si>
-    <t>Task 7 description</t>
-  </si>
-  <si>
-    <t>11/30/2024 6:30:00 PM</t>
-  </si>
-  <si>
-    <t>Task 8</t>
-  </si>
-  <si>
-    <t>12/1/2024 10:30:00 PM</t>
-  </si>
-  <si>
-    <t>Task 8 description</t>
-  </si>
-  <si>
-    <t>12/1/2024 9:55:00 PM</t>
-  </si>
-  <si>
-    <t>Task 9</t>
-  </si>
-  <si>
-    <t>11/28/2024 10:50:00 AM</t>
-  </si>
-  <si>
-    <t>Task 9 description</t>
-  </si>
-  <si>
-    <t>11/28/2024 10:15:00 AM</t>
-  </si>
-  <si>
-    <t>Task 10</t>
-  </si>
-  <si>
-    <t>11/29/2024 3:41:00 PM</t>
-  </si>
-  <si>
-    <t>Task 10 description</t>
-  </si>
-  <si>
-    <t>11/29/2024 3:12:00 PM</t>
-  </si>
-  <si>
-    <t>Task 11</t>
-  </si>
-  <si>
-    <t>11/30/2024 6:32:00 PM</t>
-  </si>
-  <si>
-    <t>Task 11 description</t>
-  </si>
-  <si>
     <t>11/30/2024 6:00:00 PM</t>
   </si>
   <si>
@@ -206,6 +179,21 @@
   </si>
   <si>
     <t>12/1/2024 8:45:00 PM</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>10/29/2024 11:59:00 PM</t>
+  </si>
+  <si>
+    <t>12/6/2024 6:00:00 AM</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>11/4/2024 11:59:00 PM</t>
   </si>
 </sst>
 </file>
@@ -594,7 +582,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
@@ -609,335 +597,335 @@
         <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="I2" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="I3" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="I4" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" s="0" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="I6" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="I7" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="E8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="I8" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="I9" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="E10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="I10" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="I11" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="I12" s="0">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I13" s="0">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#22 - ThreadPoolTimer reminder notification
</commit_message>
<xml_diff>
--- a/TimeManagementApp/Dao/tasks.xlsx
+++ b/TimeManagementApp/Dao/tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>TaskId</t>
   </si>
@@ -91,28 +91,31 @@
     <t>Task 5 description</t>
   </si>
   <si>
+    <t>12/2/2024 9:46:00 PM</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>11/29/2024 2:22:00 PM</t>
+  </si>
+  <si>
+    <t>Task 6 description</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>11/30/2024 7:05:00 PM</t>
+  </si>
+  <si>
+    <t>Task 7 description</t>
+  </si>
+  <si>
     <t>1/1/2000 1:00:00 AM</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>11/29/2024 2:22:00 PM</t>
-  </si>
-  <si>
-    <t>Task 6 description</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>11/30/2024 7:05:00 PM</t>
-  </si>
-  <si>
-    <t>Task 7 description</t>
   </si>
   <si>
     <t>Task 8</t>
@@ -719,7 +722,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I6" s="0">
         <v>7</v>
@@ -730,13 +733,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>18</v>
@@ -745,10 +748,10 @@
         <v>12</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I7" s="0">
         <v>8</v>
@@ -759,13 +762,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>12</v>
@@ -777,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I8" s="0">
         <v>9</v>
@@ -788,13 +791,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>18</v>
@@ -806,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9" s="0">
         <v>10</v>
@@ -817,13 +820,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>12</v>
@@ -832,10 +835,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I10" s="0">
         <v>11</v>
@@ -846,13 +849,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>18</v>
@@ -864,7 +867,7 @@
         <v>27</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" s="0">
         <v>12</v>
@@ -875,13 +878,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>12</v>
@@ -890,10 +893,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I12" s="0">
         <v>0</v>
@@ -904,13 +907,13 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>12</v>
@@ -919,10 +922,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I13" s="0">
         <v>0</v>

</xml_diff>